<commit_message>
Updated simultaneous ferric and influent q work
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>femass</t>
   </si>
@@ -33,9 +33,6 @@
   </si>
   <si>
     <t>femass/spo4_effl</t>
-  </si>
-  <si>
-    <t>q_infl</t>
   </si>
   <si>
     <t>q_infl/spo4_effl</t>
@@ -48,6 +45,15 @@
   </si>
   <si>
     <t>spo4_effl/q_infl</t>
+  </si>
+  <si>
+    <t>q_infl (frac change)</t>
+  </si>
+  <si>
+    <t>q_infl (actual)</t>
+  </si>
+  <si>
+    <t>q_infl (actual increase)</t>
   </si>
 </sst>
 </file>
@@ -63,12 +69,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -83,8 +95,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -170,7 +184,12 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.2668963254593115E-2"/>
+                  <c:y val="0.13913188976377952"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -211,22 +230,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.8724584499999999E-2</c:v>
+                  <c:v>1.4339669499999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.7449168999999998E-2</c:v>
+                  <c:v>2.8679338999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11617375349999999</c:v>
+                  <c:v>4.3019008499999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.154898338</c:v>
+                  <c:v>5.7358677999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.19362292249999999</c:v>
+                  <c:v>7.1698347499999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.23234750699999998</c:v>
+                  <c:v>8.6038016999999994E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -268,11 +287,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$3</c:f>
+              <c:f>Sheet1!$G$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>q_infl</c:v>
+                  <c:v>q_infl (frac change)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -346,7 +365,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$4:$F$16</c:f>
+              <c:f>Sheet1!$J$4:$J$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -354,47 +373,47 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.8964336800000003E-2</c:v>
+                  <c:v>1.5585656825E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1146538622</c:v>
+                  <c:v>3.0198511300000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.16706857619999999</c:v>
+                  <c:v>4.3838563424999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.21620847879999999</c:v>
+                  <c:v>5.6505813199999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.26207356999999998</c:v>
+                  <c:v>6.8200260624999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.3046638498</c:v>
+                  <c:v>7.8921905700000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.34397931819999999</c:v>
+                  <c:v>8.8670748424999987E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.38001997519999997</c:v>
+                  <c:v>9.7446788799999989E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.41278582080000004</c:v>
+                  <c:v>0.105250026825</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.44227685500000002</c:v>
+                  <c:v>0.11208046250000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.46849307780000005</c:v>
+                  <c:v>0.11793809582500002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.49143448919999999</c:v>
+                  <c:v>0.1228229268</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$4:$E$16</c:f>
+              <c:f>Sheet1!$G$4:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -450,11 +469,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="485801208"/>
-        <c:axId val="485799248"/>
+        <c:axId val="405764928"/>
+        <c:axId val="405755912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="485801208"/>
+        <c:axId val="405764928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -567,12 +586,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="485799248"/>
+        <c:crossAx val="405755912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="485799248"/>
+        <c:axId val="405755912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -690,7 +709,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="485801208"/>
+        <c:crossAx val="405764928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1299,16 +1318,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1593,15 +1612,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1609,22 +1628,22 @@
         <v>0</v>
       </c>
       <c r="C1">
-        <v>-0.77449168999999995</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1">
+        <v>-0.28679338999999998</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1">
         <v>0</v>
       </c>
-      <c r="G1">
-        <v>1.21203485</v>
-      </c>
-      <c r="H1">
-        <v>-0.65496228000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1">
+        <v>0.32144116</v>
+      </c>
+      <c r="J1">
+        <v>-0.19456047000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1632,16 +1651,22 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1653,189 +1678,283 @@
         <f>ABS(B4)</f>
         <v>0</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>0</v>
       </c>
-      <c r="F4">
-        <f>$F$1+E4*$G$1+E4^2*$H$1</f>
+      <c r="H4">
+        <f>G4*2788860</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <f>(1+G4)*2788860</f>
+        <v>2788860</v>
+      </c>
+      <c r="J4">
+        <f>$H$1+G4*$I$1+G4^2*$J$1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.05</v>
       </c>
       <c r="B5">
-        <f t="shared" ref="B5:B34" si="0">$B$1+A5*$C$1</f>
-        <v>-3.8724584499999999E-2</v>
+        <f t="shared" ref="B5:B10" si="0">$B$1+A5*$C$1</f>
+        <v>-1.4339669499999999E-2</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:C34" si="1">ABS(B5)</f>
-        <v>3.8724584499999999E-2</v>
-      </c>
-      <c r="E5">
+        <f t="shared" ref="C5:C10" si="1">ABS(B5)</f>
+        <v>1.4339669499999999E-2</v>
+      </c>
+      <c r="G5">
         <v>0.05</v>
       </c>
-      <c r="F5">
-        <f t="shared" ref="F5:F16" si="2">$F$1+E5*$G$1+E5^2*$H$1</f>
-        <v>5.8964336800000003E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H5">
+        <f t="shared" ref="H5:H16" si="2">G5*2788860</f>
+        <v>139443</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I16" si="3">(1+G5)*2788860</f>
+        <v>2928303</v>
+      </c>
+      <c r="J5">
+        <f>$H$1+G5*$I$1+G5^2*$J$1</f>
+        <v>1.5585656825E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0.1</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>-7.7449168999999998E-2</v>
+        <v>-2.8679338999999998E-2</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>7.7449168999999998E-2</v>
-      </c>
-      <c r="E6">
+        <v>2.8679338999999998E-2</v>
+      </c>
+      <c r="G6">
         <v>0.1</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <f t="shared" si="2"/>
-        <v>0.1146538622</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>278886</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="3"/>
+        <v>3067746.0000000005</v>
+      </c>
+      <c r="J6">
+        <f>$H$1+G6*$I$1+G6^2*$J$1</f>
+        <v>3.0198511300000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0.15</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>-0.11617375349999999</v>
+        <v>-4.3019008499999997E-2</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>0.11617375349999999</v>
-      </c>
-      <c r="E7">
+        <v>4.3019008499999997E-2</v>
+      </c>
+      <c r="G7">
         <v>0.15</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <f t="shared" si="2"/>
-        <v>0.16706857619999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>418329</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>3207188.9999999995</v>
+      </c>
+      <c r="J7">
+        <f>$H$1+G7*$I$1+G7^2*$J$1</f>
+        <v>4.3838563424999998E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0.2</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>-0.154898338</v>
+        <v>-5.7358677999999996E-2</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>0.154898338</v>
-      </c>
-      <c r="E8">
+        <v>5.7358677999999996E-2</v>
+      </c>
+      <c r="G8">
         <v>0.2</v>
       </c>
-      <c r="F8">
+      <c r="H8">
         <f t="shared" si="2"/>
-        <v>0.21620847879999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>557772</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>3346632</v>
+      </c>
+      <c r="J8">
+        <f>$H$1+G8*$I$1+G8^2*$J$1</f>
+        <v>5.6505813199999998E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0.25</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>-0.19362292249999999</v>
+        <v>-7.1698347499999995E-2</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>0.19362292249999999</v>
-      </c>
-      <c r="E9">
+        <v>7.1698347499999995E-2</v>
+      </c>
+      <c r="G9">
         <v>0.25</v>
       </c>
-      <c r="F9">
+      <c r="H9">
         <f t="shared" si="2"/>
-        <v>0.26207356999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>697215</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>3486075</v>
+      </c>
+      <c r="J9">
+        <f>$H$1+G9*$I$1+G9^2*$J$1</f>
+        <v>6.8200260624999995E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0.3</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>-0.23234750699999998</v>
+        <v>-8.6038016999999994E-2</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>0.23234750699999998</v>
-      </c>
-      <c r="E10">
+        <v>8.6038016999999994E-2</v>
+      </c>
+      <c r="G10">
         <v>0.3</v>
       </c>
-      <c r="F10">
+      <c r="H10">
         <f t="shared" si="2"/>
-        <v>0.3046638498</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E11">
+        <v>836658</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>3625518</v>
+      </c>
+      <c r="J10">
+        <f>$H$1+G10*$I$1+G10^2*$J$1</f>
+        <v>7.8921905700000003E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G11">
         <v>0.35</v>
       </c>
-      <c r="F11">
+      <c r="H11">
         <f t="shared" si="2"/>
-        <v>0.34397931819999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>976100.99999999988</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>3764961.0000000005</v>
+      </c>
+      <c r="J11">
+        <f>$H$1+G11*$I$1+G11^2*$J$1</f>
+        <v>8.8670748424999987E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12">
-        <v>1.2911999999999999</v>
-      </c>
-      <c r="E12">
+        <v>3.4868000000000001</v>
+      </c>
+      <c r="G12">
         <v>0.4</v>
       </c>
-      <c r="F12">
+      <c r="H12">
         <f t="shared" si="2"/>
-        <v>0.38001997519999997</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E13">
+        <v>1115544</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>3904403.9999999995</v>
+      </c>
+      <c r="J12">
+        <f>$H$1+G12*$I$1+G12^2*$J$1</f>
+        <v>9.7446788799999989E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G13">
         <v>0.45</v>
       </c>
-      <c r="F13">
+      <c r="H13">
         <f t="shared" si="2"/>
-        <v>0.41278582080000004</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1254987</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="3"/>
+        <v>4043847</v>
+      </c>
+      <c r="J13">
+        <f>$H$1+G13*$I$1+G13^2*$J$1</f>
+        <v>0.105250026825</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14">
         <v>0.5</v>
       </c>
-      <c r="F14">
+      <c r="H14">
         <f t="shared" si="2"/>
-        <v>0.44227685500000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1394430</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="3"/>
+        <v>4183290</v>
+      </c>
+      <c r="J14">
+        <f>$H$1+G14*$I$1+G14^2*$J$1</f>
+        <v>0.11208046250000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0</v>
       </c>
@@ -1844,203 +1963,625 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <f>$F$18+A15*$G$18+A15*$H$18</f>
+        <f>$H$18+A15*$I$18+A15^2*$J$18</f>
         <v>0</v>
       </c>
+      <c r="D15">
+        <f>C15*2788860</f>
+        <v>0</v>
+      </c>
       <c r="E15">
+        <f>(1+C15)*2788860</f>
+        <v>2788860</v>
+      </c>
+      <c r="G15">
         <v>0.55000000000000004</v>
       </c>
-      <c r="F15">
+      <c r="H15">
         <f t="shared" si="2"/>
-        <v>0.46849307780000005</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1533873.0000000002</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="3"/>
+        <v>4322733</v>
+      </c>
+      <c r="J15">
+        <f>$H$1+G15*$I$1+G15^2*$J$1</f>
+        <v>0.11793809582500002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>0.02</v>
       </c>
       <c r="B16">
-        <f t="shared" ref="B16:B28" si="3">$B$12+A16*$C$12</f>
-        <v>2.5824E-2</v>
+        <f t="shared" ref="B16:B42" si="4">$B$12+A16*$C$12</f>
+        <v>6.9736000000000006E-2</v>
       </c>
       <c r="C16">
-        <f t="shared" ref="C16:C28" si="4">$F$18+A16*$G$18+A16*$H$18</f>
-        <v>3.449E-2</v>
+        <f t="shared" ref="C16:C42" si="5">$H$18+A16*$I$18+A16^2*$J$18</f>
+        <v>5.4641599999999999E-2</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ref="D16:D42" si="6">C16*2788860</f>
+        <v>152387.77257599999</v>
       </c>
       <c r="E16">
+        <f t="shared" ref="E16:E42" si="7">(1+C16)*2788860</f>
+        <v>2941247.7725760001</v>
+      </c>
+      <c r="G16">
         <v>0.6</v>
       </c>
-      <c r="F16">
+      <c r="H16">
         <f t="shared" si="2"/>
-        <v>0.49143448919999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1673316</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="3"/>
+        <v>4462176</v>
+      </c>
+      <c r="J16">
+        <f>$H$1+G16*$I$1+G16^2*$J$1</f>
+        <v>0.1228229268</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>0.04</v>
       </c>
       <c r="B17">
-        <f t="shared" si="3"/>
-        <v>5.1647999999999999E-2</v>
+        <f t="shared" si="4"/>
+        <v>0.13947200000000001</v>
       </c>
       <c r="C17">
-        <f t="shared" si="4"/>
-        <v>6.898E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+        <f t="shared" si="5"/>
+        <v>0.12474640000000001</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="6"/>
+        <v>347900.24510400003</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="7"/>
+        <v>3136760.245104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>0.06</v>
       </c>
       <c r="B18">
-        <f t="shared" si="3"/>
-        <v>7.7471999999999985E-2</v>
+        <f t="shared" si="4"/>
+        <v>0.20920800000000001</v>
       </c>
       <c r="C18">
+        <f t="shared" si="5"/>
+        <v>0.21031440000000001</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="6"/>
+        <v>586537.41758400004</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="7"/>
+        <v>3375397.4175840002</v>
+      </c>
+      <c r="G18" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>2.3454999999999999</v>
+      </c>
+      <c r="J18">
+        <v>19.329000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="B19" s="1">
         <f t="shared" si="4"/>
-        <v>0.10346999999999998</v>
-      </c>
-      <c r="E18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0.67749999999999999</v>
-      </c>
-      <c r="H18">
-        <v>1.0469999999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>0.08</v>
-      </c>
-      <c r="B19">
-        <f t="shared" si="3"/>
-        <v>0.103296</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="4"/>
-        <v>0.13796</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0.27894400000000003</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="5"/>
+        <v>0.3113456</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="6"/>
+        <v>868299.29001600004</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="7"/>
+        <v>3657159.2900160002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>0.1</v>
       </c>
       <c r="B20">
-        <f t="shared" si="3"/>
-        <v>0.12911999999999998</v>
+        <f t="shared" si="4"/>
+        <v>0.34868000000000005</v>
       </c>
       <c r="C20">
+        <f t="shared" si="5"/>
+        <v>0.42784000000000005</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="6"/>
+        <v>1193185.8624000002</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="7"/>
+        <v>3982045.8624</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="B21" s="2">
         <f t="shared" si="4"/>
-        <v>0.17244999999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>0.12</v>
-      </c>
-      <c r="B21">
-        <f t="shared" si="3"/>
-        <v>0.15494399999999997</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="4"/>
-        <v>0.20693999999999996</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0.41841600000000001</v>
+      </c>
+      <c r="C21" s="2">
+        <f t="shared" si="5"/>
+        <v>0.55979760000000001</v>
+      </c>
+      <c r="D21" s="2">
+        <f t="shared" si="6"/>
+        <v>1561197.1347360001</v>
+      </c>
+      <c r="E21" s="2">
+        <f t="shared" si="7"/>
+        <v>4350057.1347359996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>0.14000000000000001</v>
       </c>
       <c r="B22">
-        <f t="shared" si="3"/>
-        <v>0.18076800000000001</v>
+        <f t="shared" si="4"/>
+        <v>0.48815200000000009</v>
       </c>
       <c r="C22">
+        <f t="shared" si="5"/>
+        <v>0.70721840000000014</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="6"/>
+        <v>1972333.1070240005</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="7"/>
+        <v>4761193.107024</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="B23" s="1">
         <f t="shared" si="4"/>
-        <v>0.24143000000000003</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>0.16</v>
-      </c>
-      <c r="B23">
-        <f t="shared" si="3"/>
-        <v>0.206592</v>
-      </c>
-      <c r="C23">
-        <f t="shared" si="4"/>
-        <v>0.27592</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0.55788800000000005</v>
+      </c>
+      <c r="C23" s="1">
+        <f t="shared" si="5"/>
+        <v>0.87010240000000005</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="6"/>
+        <v>2426593.7792640002</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="7"/>
+        <v>5215453.7792640002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>0.18</v>
       </c>
       <c r="B24">
-        <f t="shared" si="3"/>
-        <v>0.23241599999999998</v>
+        <f t="shared" si="4"/>
+        <v>0.62762399999999996</v>
       </c>
       <c r="C24">
+        <f t="shared" si="5"/>
+        <v>1.0484496000000001</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="6"/>
+        <v>2923979.1514560003</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="7"/>
+        <v>5712839.1514560003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="B25" s="2">
         <f t="shared" si="4"/>
-        <v>0.31040999999999996</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>0.2</v>
-      </c>
-      <c r="B25">
-        <f t="shared" si="3"/>
-        <v>0.25823999999999997</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="4"/>
-        <v>0.34489999999999998</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0.69736000000000009</v>
+      </c>
+      <c r="C25" s="2">
+        <f t="shared" si="5"/>
+        <v>1.2422600000000001</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" si="6"/>
+        <v>3464489.2236000006</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" si="7"/>
+        <v>6253349.2236000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>0.22</v>
       </c>
       <c r="B26">
-        <f t="shared" si="3"/>
-        <v>0.28406399999999998</v>
+        <f t="shared" si="4"/>
+        <v>0.767096</v>
       </c>
       <c r="C26">
+        <f t="shared" si="5"/>
+        <v>1.4515335999999999</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="6"/>
+        <v>4048123.9956959998</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="7"/>
+        <v>6836983.9956959998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="B27" s="1">
         <f t="shared" si="4"/>
-        <v>0.37939000000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>0.24</v>
-      </c>
-      <c r="B27">
-        <f t="shared" si="3"/>
-        <v>0.30988799999999994</v>
-      </c>
-      <c r="C27">
-        <f t="shared" si="4"/>
-        <v>0.41387999999999991</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0.83683200000000002</v>
+      </c>
+      <c r="C27" s="1">
+        <f t="shared" si="5"/>
+        <v>1.6762703999999999</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="6"/>
+        <v>4674883.4677440003</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="7"/>
+        <v>7463743.4677440003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>0.26</v>
       </c>
       <c r="B28">
-        <f t="shared" si="3"/>
-        <v>0.33571200000000001</v>
+        <f t="shared" si="4"/>
+        <v>0.90656800000000004</v>
       </c>
       <c r="C28">
+        <f t="shared" si="5"/>
+        <v>1.9164704000000001</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="6"/>
+        <v>5344767.6397440005</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="7"/>
+        <v>8133627.6397440005</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="B29" s="1">
         <f t="shared" si="4"/>
-        <v>0.44837000000000005</v>
+        <v>0.97630400000000017</v>
+      </c>
+      <c r="C29" s="1">
+        <f t="shared" si="5"/>
+        <v>2.1721336000000004</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="6"/>
+        <v>6057776.5116960015</v>
+      </c>
+      <c r="E29" s="1">
+        <f t="shared" si="7"/>
+        <v>8846636.5116960015</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>0.3</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="4"/>
+        <v>1.0460400000000001</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="5"/>
+        <v>2.44326</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="6"/>
+        <v>6813910.0835999995</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="7"/>
+        <v>9602770.0835999995</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>0.32</v>
+      </c>
+      <c r="B31" s="2">
+        <f t="shared" si="4"/>
+        <v>1.1157760000000001</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" si="5"/>
+        <v>2.7298496000000001</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" si="6"/>
+        <v>7613168.3554560002</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="7"/>
+        <v>10402028.355456</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>0.36</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="4"/>
+        <v>1.2552479999999999</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="5"/>
+        <v>3.3494184000000002</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="6"/>
+        <v>9341058.999024</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="7"/>
+        <v>12129918.999024</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="B33" s="1">
+        <f t="shared" si="4"/>
+        <v>1.3947200000000002</v>
+      </c>
+      <c r="C33" s="1">
+        <f t="shared" si="5"/>
+        <v>4.0308400000000004</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="6"/>
+        <v>11241448.442400001</v>
+      </c>
+      <c r="E33" s="1">
+        <f t="shared" si="7"/>
+        <v>14030308.442400001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>0.44</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="4"/>
+        <v>1.534192</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="5"/>
+        <v>4.7741144000000002</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="6"/>
+        <v>13314336.685584001</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="7"/>
+        <v>16103196.685584001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="B35" s="1">
+        <f t="shared" si="4"/>
+        <v>1.673664</v>
+      </c>
+      <c r="C35" s="1">
+        <f t="shared" si="5"/>
+        <v>5.5792416000000005</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="6"/>
+        <v>15559723.728576001</v>
+      </c>
+      <c r="E35" s="1">
+        <f t="shared" si="7"/>
+        <v>18348583.728576001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>0.54</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="4"/>
+        <v>1.8828720000000001</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="5"/>
+        <v>6.9029064</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="6"/>
+        <v>19251239.542704001</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="7"/>
+        <v>22040099.542704001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="B37" s="1">
+        <f t="shared" si="4"/>
+        <v>2.0920800000000002</v>
+      </c>
+      <c r="C37" s="1">
+        <f t="shared" si="5"/>
+        <v>8.3657400000000006</v>
+      </c>
+      <c r="D37" s="1">
+        <f t="shared" si="6"/>
+        <v>23330877.656400003</v>
+      </c>
+      <c r="E37" s="1">
+        <f t="shared" si="7"/>
+        <v>26119737.656400003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>0.66</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="4"/>
+        <v>2.301288</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="5"/>
+        <v>9.9677424000000023</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="6"/>
+        <v>27798638.069664005</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="7"/>
+        <v>30587498.069664005</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="B39" s="1">
+        <f t="shared" si="4"/>
+        <v>2.5104959999999998</v>
+      </c>
+      <c r="C39" s="1">
+        <f t="shared" si="5"/>
+        <v>11.708913600000001</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" si="6"/>
+        <v>32654520.782496002</v>
+      </c>
+      <c r="E39" s="1">
+        <f t="shared" si="7"/>
+        <v>35443380.782496005</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>0.8</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="4"/>
+        <v>2.7894400000000004</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="5"/>
+        <v>14.246960000000003</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="6"/>
+        <v>39732776.865600012</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="7"/>
+        <v>42521636.865600012</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="B41" s="1">
+        <f t="shared" si="4"/>
+        <v>3.068384</v>
+      </c>
+      <c r="C41" s="1">
+        <f t="shared" si="5"/>
+        <v>17.032417599999999</v>
+      </c>
+      <c r="D41" s="1">
+        <f t="shared" si="6"/>
+        <v>47501028.147935994</v>
+      </c>
+      <c r="E41" s="1">
+        <f t="shared" si="7"/>
+        <v>50289888.147935994</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>1</v>
+      </c>
+      <c r="B42" s="1">
+        <f t="shared" si="4"/>
+        <v>3.4868000000000001</v>
+      </c>
+      <c r="C42" s="1">
+        <f t="shared" si="5"/>
+        <v>21.674500000000002</v>
+      </c>
+      <c r="D42" s="1">
+        <f t="shared" si="6"/>
+        <v>60447146.070000008</v>
+      </c>
+      <c r="E42" s="1">
+        <f t="shared" si="7"/>
+        <v>63236006.070000008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>